<commit_message>
bot_eleitor - API + Excel funcionou
</commit_message>
<xml_diff>
--- a/bot_eleitor/resources/RelacaoEleitor.xlsx
+++ b/bot_eleitor/resources/RelacaoEleitor.xlsx
@@ -13,14 +13,14 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t xml:space="preserve">CPF</t>
   </si>
@@ -40,43 +40,80 @@
     <t xml:space="preserve">NRO_ENDERECO</t>
   </si>
   <si>
-    <t xml:space="preserve">BENEVALDO PEREIRA GONCALVES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROSA NUNES PEREIRA GONCALVES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">69086486</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8045</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BRUNO PEREIRA GONCALVES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">69415000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8044</t>
+    <t xml:space="preserve">01664388206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LUCAS DA ROCHA ANDRADE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELIANA BEZERRA DA ROCHA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69033620</t>
+  </si>
+  <si>
+    <t xml:space="preserve">728</t>
+  </si>
+  <si>
+    <t xml:space="preserve">70390243221</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CARLOS VINICIUS MONTEIRO DE SOUZA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGDA MONTEIRO DE SOUZA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69054691</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03525405243</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAIO CESAR FANECO GONZAGA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LILIAN CRISTINA ANDRADE FANECO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69093200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04981577257</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NELSON THIAGO DA SILVA PINTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LUCILENE BALIEIRO DA SILVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69085200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">393</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0"/>
+    <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="d/m/yyyy"/>
-    <numFmt numFmtId="167" formatCode="@"/>
-    <numFmt numFmtId="168" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -94,20 +131,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -152,60 +175,36 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -222,7 +221,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -256,20 +255,20 @@
         <a:srgbClr val="4ea72e"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000ff"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="96607d"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -283,52 +282,63 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
+                <a:lumMod val="110000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
-              <a:schemeClr val="phClr"/>
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
           <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="51000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="94000"/>
+                <a:lumMod val="99000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
           <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -346,44 +356,34 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
+                <a:tint val="93000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="20000"/>
+                <a:shade val="63000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
           <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -397,93 +397,127 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="18.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="38.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="41.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="5" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="5" width="15.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="18.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="38.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="41.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="15.89"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+    <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="n">
-        <v>93337205291</v>
-      </c>
-      <c r="B2" s="7" t="n">
-        <v>27236.0000462963</v>
-      </c>
-      <c r="C2" s="11" t="s">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="B2" s="5" t="n">
+        <v>34247</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="F2" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="n">
-        <v>53876549806</v>
-      </c>
-      <c r="B3" s="7" t="n">
-        <v>31620.0000462963</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="9" t="s">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="B3" s="5" t="n">
+        <v>36905</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="D3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E6" s="12"/>
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>36278</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="7" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C7" s="13"/>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>37985</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>